<commit_message>
UI text Name of Rico
</commit_message>
<xml_diff>
--- a/CHATGAME/Assets/StreamingAssets/Excel/UI text.xlsx
+++ b/CHATGAME/Assets/StreamingAssets/Excel/UI text.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\one\Desktop\AIChatGame\AI-CHATBOT-GAME\CHATGAME\Assets\StreamingAssets\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2E87E8E3-3683-4996-8D6B-9A36301E1F45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C5550308-FD33-49A2-A998-47F8469968C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1830" yWindow="765" windowWidth="19470" windowHeight="13245" xr2:uid="{52C131E0-3625-409F-9DBC-C4D8ECB4944A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="64">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -523,6 +523,12 @@
   </si>
   <si>
     <t>Event</t>
+  </si>
+  <si>
+    <t>리코</t>
+  </si>
+  <si>
+    <t>Rico</t>
   </si>
   <si>
     <t>EOF</t>
@@ -1185,10 +1191,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E05533CD-8686-4012-9E6D-F284907C7539}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="13.5"/>
@@ -1473,9 +1479,26 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
-      <c r="A17" s="1" t="s">
+    <row r="17" spans="1:5">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>61</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Good Good very Good
</commit_message>
<xml_diff>
--- a/CHATGAME/Assets/StreamingAssets/Excel/UI text.xlsx
+++ b/CHATGAME/Assets/StreamingAssets/Excel/UI text.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\one\Desktop\AIChatGame\AI-CHATBOT-GAME\CHATGAME\Assets\StreamingAssets\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C5550308-FD33-49A2-A998-47F8469968C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7B443C94-7D36-4CC2-A087-C9183D8BA723}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1830" yWindow="765" windowWidth="19470" windowHeight="13245" xr2:uid="{52C131E0-3625-409F-9DBC-C4D8ECB4944A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="68">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -529,6 +529,18 @@
   </si>
   <si>
     <t>Rico</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
   </si>
   <si>
     <t>EOF</t>
@@ -1191,10 +1203,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E05533CD-8686-4012-9E6D-F284907C7539}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="13.5"/>
@@ -1497,8 +1509,25 @@
       </c>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>63</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>